<commit_message>
Fix up PC proposal template
</commit_message>
<xml_diff>
--- a/Resources/Guidelines/sigplan-pc-proposal-template.xlsx
+++ b/Resources/Guidelines/sigplan-pc-proposal-template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bcpierce/current/sigplan/documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bcpierce/home/SIGPLAN.github.io/Resources/Guidelines/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9921DB8B-BF28-CE48-8AA9-D99E49F4A2D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C91B12B-B8DC-3B4C-BE8F-22FAC7E56023}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>First Name</t>
   </si>
@@ -64,18 +64,12 @@
     <t>www.jim.com</t>
   </si>
   <si>
-    <t>PhD year</t>
-  </si>
-  <si>
     <t>Areas of Expertise</t>
   </si>
   <si>
     <t>Bourbon, single malts</t>
   </si>
   <si>
-    <t>SIGPLAN Conference / Workshop Planner</t>
-  </si>
-  <si>
     <t>Last served on this PC</t>
   </si>
   <si>
@@ -116,13 +110,31 @@
   </si>
   <si>
     <t>Additional comments</t>
+  </si>
+  <si>
+    <t>Please start by reading the instructions:</t>
+  </si>
+  <si>
+    <t>SIGPLAN PC Proposal</t>
+  </si>
+  <si>
+    <t>&lt;fill in here&gt;</t>
+  </si>
+  <si>
+    <t>Approximate year of PhD</t>
+  </si>
+  <si>
+    <t>https://www.sigplan.org/Resources/Guidelines/ProposalInstructions/</t>
+  </si>
+  <si>
+    <t>Conference / Workshop:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -144,13 +156,6 @@
       <name val="Arial"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -176,6 +181,34 @@
     </font>
     <font>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="4"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -214,9 +247,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -225,16 +258,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -243,28 +273,40 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -283,130 +325,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>203200</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>114301</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>1456267</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>59267</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F700814-B2F2-4646-B307-8C6279B558D2}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="203200" y="410634"/>
-          <a:ext cx="9457267" cy="2197100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>Instructions</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>:</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>- This spreadsheet is intended both to help PC Chairs review the coverage and diversity of proposed</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> PCs and to help the SIGPLAN EC quickly evaluate and approve proposals.  </a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>- Please begin by having a look at SIGPLAN's diversity policy at http://www.sigplan.org/Resources/Policies/Diversity/</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>-</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> Workshop PCs may include at most one PhD student in their final year; please include a comment detailing their qualifications.  Conference PC members should all have PhDs by the submission deadline.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>- For PC members in industry jobs (except industrial research labs), please include a comment on their reviewing experience and publications.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>- To expedite forming the PC, make sure you've chosen some alternate PC members, to be invited in case someone in the "first round" declines to serve.   Use the "Invite now or keep as alternate" column to indicate which is which.  You may also find it useful to make notes in the Comments column about who a given alternate might replace.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>- Use the "Connection to organizers" column to note close connections between proposed PC members and the organizers of the conference (e.g., former advisor, student, or postdoc, same institution, etc.) -- especially with the PC chair(s).</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -709,11 +627,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:W8"/>
+  <dimension ref="A1:W10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -723,12 +641,12 @@
     <col min="3" max="3" width="16.5" style="2" customWidth="1"/>
     <col min="4" max="4" width="8.1640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="7.5" style="2" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11" style="2" customWidth="1"/>
     <col min="7" max="7" width="10.33203125" style="2" customWidth="1"/>
     <col min="8" max="8" width="17.6640625" style="2" customWidth="1"/>
     <col min="9" max="9" width="22.5" style="2" customWidth="1"/>
     <col min="10" max="10" width="17.1640625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="1.33203125" style="9" customWidth="1"/>
+    <col min="11" max="11" width="1.33203125" style="8" customWidth="1"/>
     <col min="12" max="12" width="18.33203125" style="2" customWidth="1"/>
     <col min="13" max="13" width="17.33203125" style="2" customWidth="1"/>
     <col min="14" max="14" width="15.5" style="2" customWidth="1"/>
@@ -737,148 +655,164 @@
   <sheetData>
     <row r="1" spans="1:23" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="4" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="3" spans="1:23" s="16" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" s="18"/>
+      <c r="L3" s="16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="151" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="3" spans="1:23" s="12" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="K3" s="13"/>
-      <c r="L3" s="12" t="s">
-        <v>19</v>
-      </c>
+    <row r="4" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="5" spans="1:23" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="20"/>
     </row>
-    <row r="4" spans="1:23" s="8" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="5" t="s">
+    <row r="6" spans="1:23" s="7" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F6" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" s="9"/>
+      <c r="L6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="K4" s="10"/>
-      <c r="L4" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="M4" s="5" t="s">
+      <c r="M6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="N6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
-      <c r="U4" s="5"/>
-      <c r="V4" s="5"/>
-      <c r="W4" s="5"/>
-    </row>
-    <row r="5" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="3">
-        <v>2007</v>
-      </c>
-      <c r="G5" s="16">
-        <v>2013</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5" s="3"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="M5" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="N5" s="16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="3">
-        <v>1998</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>21</v>
-      </c>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
     </row>
     <row r="7" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="F7" s="3"/>
-      <c r="I7" s="3"/>
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="3">
+        <v>2007</v>
+      </c>
+      <c r="G7" s="13">
+        <v>2013</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="3"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="M7" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="N7" s="13" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="F8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
+      <c r="A8" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1998</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F9" s="3"/>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N5" r:id="rId1" xr:uid="{EB85A920-7597-084E-AC55-8AEAC31564BD}"/>
+    <hyperlink ref="N7" r:id="rId1" xr:uid="{EB85A920-7597-084E-AC55-8AEAC31564BD}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{57BC6453-C0EB-C043-9C48-7DB25E8698E0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
More updates to proposal instructions
</commit_message>
<xml_diff>
--- a/Resources/Guidelines/sigplan-pc-proposal-template.xlsx
+++ b/Resources/Guidelines/sigplan-pc-proposal-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bcpierce/home/SIGPLAN.github.io/Resources/Guidelines/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C91B12B-B8DC-3B4C-BE8F-22FAC7E56023}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1ED3878-1095-9646-9C78-6F7269DD384A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>First Name</t>
   </si>
@@ -127,14 +127,39 @@
     <t>https://www.sigplan.org/Resources/Guidelines/ProposalInstructions/</t>
   </si>
   <si>
-    <t>Conference / Workshop:</t>
+    <t>Conference or workshop name:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Main conference </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(if this is a workshop or co-located event)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>:</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -209,6 +234,13 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -627,18 +659,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:W10"/>
+  <dimension ref="A1:W12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12.5" style="2" customWidth="1"/>
     <col min="2" max="2" width="14.5" style="2"/>
-    <col min="3" max="3" width="16.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="8.1640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="7.5" style="2" customWidth="1"/>
     <col min="6" max="6" width="11" style="2" customWidth="1"/>
@@ -667,149 +699,163 @@
         <v>34</v>
       </c>
       <c r="K3" s="18"/>
-      <c r="L3" s="16" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="4" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="5" spans="1:23" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="E5" s="19" t="s">
         <v>32</v>
       </c>
       <c r="K5" s="20"/>
-    </row>
-    <row r="6" spans="1:23" s="7" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="5" t="s">
+      <c r="L5" s="16"/>
+    </row>
+    <row r="6" spans="1:23" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="K6" s="20"/>
+      <c r="L6" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" s="19" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K7" s="20"/>
+      <c r="L7" s="16"/>
+    </row>
+    <row r="8" spans="1:23" s="7" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B8" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F8" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H8" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="J8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="K6" s="9"/>
-      <c r="L6" s="6" t="s">
+      <c r="K8" s="9"/>
+      <c r="L8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="M8" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="N6" s="5" t="s">
+      <c r="N8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="5"/>
-      <c r="T6" s="5"/>
-      <c r="U6" s="5"/>
-      <c r="V6" s="5"/>
-      <c r="W6" s="5"/>
-    </row>
-    <row r="7" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="3" t="s">
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+    </row>
+    <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F9" s="3">
         <v>2007</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G9" s="13">
         <v>2013</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="13" t="s">
+      <c r="J9" s="3"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="M7" s="14" t="s">
+      <c r="M9" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="N7" s="13" t="s">
+      <c r="N9" s="13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="12" t="s">
+    <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B10" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C10" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D10" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E10" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F10" s="3">
         <v>1998</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G10" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="H10" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I10" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="F9" s="3"/>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="F10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
+    <row r="11" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F11" s="3"/>
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N7" r:id="rId1" xr:uid="{EB85A920-7597-084E-AC55-8AEAC31564BD}"/>
+    <hyperlink ref="N9" r:id="rId1" xr:uid="{EB85A920-7597-084E-AC55-8AEAC31564BD}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{57BC6453-C0EB-C043-9C48-7DB25E8698E0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Tweak to PC proposal template
</commit_message>
<xml_diff>
--- a/Resources/Guidelines/sigplan-pc-proposal-template.xlsx
+++ b/Resources/Guidelines/sigplan-pc-proposal-template.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bcpierce/home/SIGPLAN.github.io/Resources/Guidelines/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1ED3878-1095-9646-9C78-6F7269DD384A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CDB4F3E-6166-5343-AC3C-AF3989F55AF9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t>First Name</t>
   </si>
@@ -112,9 +112,6 @@
     <t>Additional comments</t>
   </si>
   <si>
-    <t>Please start by reading the instructions:</t>
-  </si>
-  <si>
     <t>SIGPLAN PC Proposal</t>
   </si>
   <si>
@@ -125,9 +122,6 @@
   </si>
   <si>
     <t>https://www.sigplan.org/Resources/Guidelines/ProposalInstructions/</t>
-  </si>
-  <si>
-    <t>Conference or workshop name:</t>
   </si>
   <si>
     <r>
@@ -154,6 +148,15 @@
       <t>:</t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve">PC Chair: </t>
+  </si>
+  <si>
+    <t>Please start by reading these instructions…</t>
+  </si>
+  <si>
+    <t>Full name (and acronym) of conference or workshop:</t>
+  </si>
 </sst>
 </file>
 
@@ -225,13 +228,6 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
@@ -242,6 +238,14 @@
       <b/>
       <sz val="9"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -329,16 +333,16 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -659,11 +663,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:W12"/>
+  <dimension ref="A1:W13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -687,175 +691,184 @@
   <sheetData>
     <row r="1" spans="1:23" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="4" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="3" spans="1:23" s="16" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="17"/>
+    </row>
+    <row r="4" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="5" spans="1:23" s="18" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" s="19"/>
+      <c r="L5" s="16"/>
+    </row>
+    <row r="6" spans="1:23" s="18" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="K3" s="18"/>
-    </row>
-    <row r="4" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="5" spans="1:23" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="19" t="s">
+      <c r="E6" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="K6" s="19"/>
+      <c r="L6" s="16"/>
+    </row>
+    <row r="7" spans="1:23" s="18" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E7" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7" s="19"/>
+    </row>
+    <row r="8" spans="1:23" s="18" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K8" s="19"/>
+      <c r="L8" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" s="7" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="K5" s="20"/>
-      <c r="L5" s="16"/>
-    </row>
-    <row r="6" spans="1:23" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="K6" s="20"/>
-      <c r="L6" s="16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" s="19" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K7" s="20"/>
-      <c r="L7" s="16"/>
-    </row>
-    <row r="8" spans="1:23" s="7" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" s="6" t="s">
+      <c r="G9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="I9" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J9" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="K8" s="9"/>
-      <c r="L8" s="6" t="s">
+      <c r="K9" s="9"/>
+      <c r="L9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="M8" s="5" t="s">
+      <c r="M9" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="N8" s="5" t="s">
+      <c r="N9" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="5"/>
-      <c r="U8" s="5"/>
-      <c r="V8" s="5"/>
-      <c r="W8" s="5"/>
-    </row>
-    <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="3" t="s">
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+    </row>
+    <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F10" s="3">
         <v>2007</v>
       </c>
-      <c r="G9" s="13">
+      <c r="G10" s="13">
         <v>2013</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="H10" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="J9" s="3"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="13" t="s">
+      <c r="J10" s="3"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="M9" s="14" t="s">
+      <c r="M10" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="N9" s="13" t="s">
+      <c r="N10" s="13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="12" t="s">
+    <row r="11" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C11" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D11" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E11" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F11" s="3">
         <v>1998</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="G11" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="H10" s="12" t="s">
+      <c r="H11" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I11" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="F11" s="3"/>
-      <c r="I11" s="3"/>
     </row>
     <row r="12" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F12" s="3"/>
       <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N9" r:id="rId1" xr:uid="{EB85A920-7597-084E-AC55-8AEAC31564BD}"/>
+    <hyperlink ref="N10" r:id="rId1" xr:uid="{EB85A920-7597-084E-AC55-8AEAC31564BD}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{57BC6453-C0EB-C043-9C48-7DB25E8698E0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>